<commit_message>
gotten as far as I can get. Believe next step is to actually properly validate, but believe I will go over this with teams
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results.csv/E/AngVel/f10RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results.csv/E/AngVel/f10RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Simulator_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results.csv\E\AngVel\f10RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF7D8FA-2F53-4333-98EB-962B9F04C46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D463AAE-A9D6-4463-BD8C-623D766D820A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9413" xr2:uid="{F8FE6B3F-D28B-4A31-B6B7-95E773C490BB}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9413" xr2:uid="{A201DA66-9083-4856-A64E-13FC6E7189A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554B7072-1291-489B-BE1F-B727C1706738}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49430C26-C264-4D42-98F6-A3358FAE3883}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>